<commit_message>
Perform data cleaning for U.S. Presidents data analysis
</commit_message>
<xml_diff>
--- a/Charts.xlsx
+++ b/Charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thonyalope\Documents\GitHub\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAB2B3A-0892-4D7B-A475-9656EC9295AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4954C3-D55E-4365-8DE5-F55279FEEA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="2370" windowWidth="28800" windowHeight="11295" activeTab="1" xr2:uid="{03CEABDE-3C67-4836-9FDD-609F2D7E7F08}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{03CEABDE-3C67-4836-9FDD-609F2D7E7F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="3" r:id="rId1"/>
@@ -150,11 +150,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6425,71 +6431,71 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="5" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>